<commit_message>
Update Sprint Plan & Retorspective.xlsx
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Sprint Plan & Retorspective.xlsx
+++ b/Documents/Agile Documents/Sprint Plan & Retorspective.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2cartj31\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39B4602-1DCA-4CA2-9397-3FAA0764C6DB}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="54">
   <si>
     <t>Sprint #1</t>
   </si>
@@ -170,12 +169,30 @@
   </si>
   <si>
     <t>Fix Dialogue</t>
+  </si>
+  <si>
+    <t>Members who were able to work on their tasks managed to get the majority if not all their work doe within in the sprint</t>
+  </si>
+  <si>
+    <t>All members can do their best to communicate when unable to do work so others may make up the difference before the sprint finishes.</t>
+  </si>
+  <si>
+    <t>Task estimates will be done with a points system to gauge the best estimates for each task. The team's velocity will also be determined next sprint.</t>
+  </si>
+  <si>
+    <t>members could try to find some more motivation towards the project as there is only 3 more sprints to go</t>
+  </si>
+  <si>
+    <t>Not much really, team motivation was down due to the repetitive nature of the project</t>
+  </si>
+  <si>
+    <t>the group will try to finish up older tasks in the next sprint, delaying the final event to sprint 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -229,7 +246,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,6 +283,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -580,10 +606,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -991,11 +1017,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D6"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1044,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="11" t="s">
@@ -1031,9 +1057,32 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
         <v>8</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Retrospective for sprint 4 added
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Sprint Plan & Retorspective.xlsx
+++ b/Documents/Agile Documents/Sprint Plan & Retorspective.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2cartj31\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\2cartj31\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="65">
   <si>
     <t>Sprint #1</t>
   </si>
@@ -189,9 +189,6 @@
     <t>the group will try to finish up older tasks in the next sprint, delaying the final event to sprint 5</t>
   </si>
   <si>
-    <t>Sprinty #4</t>
-  </si>
-  <si>
     <t>Catchup on work so Final event can be started</t>
   </si>
   <si>
@@ -208,6 +205,21 @@
   </si>
   <si>
     <t xml:space="preserve">Save Game Script </t>
+  </si>
+  <si>
+    <t>Sprint #4</t>
+  </si>
+  <si>
+    <t>Sprint #5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The team managed to get under the ideal burndown for the first few days in this sprint </t>
+  </si>
+  <si>
+    <t>members are still rather demotivated on the project, which is to be expected at this late stage</t>
+  </si>
+  <si>
+    <t>the group needs to just make sure the essential work gets done, the aim of the next two sprints is to achieve that</t>
   </si>
 </sst>
 </file>
@@ -223,7 +235,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,6 +266,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -267,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -314,10 +332,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,8 +655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -961,10 +982,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="20" t="s">
         <v>54</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>55</v>
       </c>
       <c r="C26" s="13" t="s">
         <v>6</v>
@@ -976,12 +997,12 @@
         <v>44</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="12"/>
-      <c r="B27" s="18"/>
+      <c r="B27" s="20"/>
       <c r="C27" s="13"/>
       <c r="D27" s="13" t="s">
         <v>37</v>
@@ -990,7 +1011,7 @@
         <v>41</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1004,7 +1025,7 @@
         <v>46</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1016,7 +1037,7 @@
         <v>14</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1028,7 +1049,7 @@
         <v>11</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1042,12 +1063,14 @@
       <c r="F31" s="13"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="19"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="7"/>
+      <c r="A32" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="19"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="1"/>
@@ -1089,8 +1112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:D7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1154,13 +1177,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Just some document changes
</commit_message>
<xml_diff>
--- a/Documents/Agile Documents/Sprint Plan & Retorspective.xlsx
+++ b/Documents/Agile Documents/Sprint Plan & Retorspective.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\SWEG-MT-Project-PT2\Documents\Agile Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\J\Desktop\Jonathan Carter SWEG-MT AE2 Submission\Individual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39B2133-15E8-44CF-A27A-B294BFA5727F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFCC6137-0771-41A6-B766-664D16ED605C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
   <si>
     <t>Sprint #1</t>
   </si>
@@ -251,6 +251,15 @@
   </si>
   <si>
     <t>Analysis of  Final Event</t>
+  </si>
+  <si>
+    <t>The team got the testing plan made and began testing each room</t>
+  </si>
+  <si>
+    <t>motivation was at an all time low. This is likely due to the projects overall scope and the amount of time we had left making people feel burned out. Considering the project was started 12 weeks ago it makes sense, considering how much needs doing.</t>
+  </si>
+  <si>
+    <t>As this was a last sprint, there isn't much to put here, but if we were to have another  sprint we would try to improve team motivation and work on little bits at a time to finish to project</t>
   </si>
 </sst>
 </file>
@@ -310,7 +319,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -359,6 +368,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,7 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -1181,10 +1193,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A3:D7"/>
+  <dimension ref="A3:D8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1262,6 +1274,20 @@
         <v>64</v>
       </c>
     </row>
+    <row r="8" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>